<commit_message>
:rocket: Real Final Deploy
</commit_message>
<xml_diff>
--- a/server/20대_개표현황.xlsx
+++ b/server/20대_개표현황.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimtaehyeong/Desktop/presidential-election/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5A6039-8AB3-9847-BB43-3462C9E463F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C49AB3C-E327-EC4C-9D46-C14980CBA009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="전국" sheetId="1" r:id="rId1"/>
@@ -1205,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1269,52 +1269,52 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q2">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1322,52 +1322,52 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1375,52 +1375,52 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1428,52 +1428,52 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1481,52 +1481,52 @@
         <v>23</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1534,52 +1534,52 @@
         <v>24</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1587,52 +1587,52 @@
         <v>25</v>
       </c>
       <c r="B8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1640,52 +1640,52 @@
         <v>26</v>
       </c>
       <c r="B9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1693,52 +1693,52 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1746,52 +1746,52 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1799,52 +1799,52 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1852,52 +1852,52 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1905,52 +1905,52 @@
         <v>31</v>
       </c>
       <c r="B14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1958,52 +1958,52 @@
         <v>32</v>
       </c>
       <c r="B15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2011,52 +2011,52 @@
         <v>33</v>
       </c>
       <c r="B16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2064,52 +2064,52 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2117,52 +2117,52 @@
         <v>35</v>
       </c>
       <c r="B18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2170,52 +2170,52 @@
         <v>36</v>
       </c>
       <c r="B19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12587,7 +12587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>

</xml_diff>